<commit_message>
code fixed and all audio are runned and saved
</commit_message>
<xml_diff>
--- a/exports/emotion_scores_comparison_id_001_pos.xlsx
+++ b/exports/emotion_scores_comparison_id_001_pos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.144</v>
+        <v>0.15</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.451</v>
+        <v>0.47</v>
       </c>
       <c r="C3" t="n">
         <v>0.9</v>
@@ -483,7 +483,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.127</v>
+        <v>0.13</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.095</v>
+        <v>0.1</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -505,27 +505,14 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Disgust</t>
+          <t>Surprise</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.055</v>
+        <v>0.14</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Surprise</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0.128</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>